<commit_message>
Add source code, edit budget
</commit_message>
<xml_diff>
--- a/2018_Documentation/Proposal, Budget, Project Schedule/Budget.xlsx
+++ b/2018_Documentation/Proposal, Budget, Project Schedule/Budget.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>No</t>
   </si>
@@ -109,6 +109,27 @@
   </si>
   <si>
     <t>Subtotal</t>
+  </si>
+  <si>
+    <t>6-pin Headers</t>
+  </si>
+  <si>
+    <t>Creatron Inc</t>
+  </si>
+  <si>
+    <t>To solder sensor into PCB</t>
+  </si>
+  <si>
+    <t>2x20 pin Headers</t>
+  </si>
+  <si>
+    <t>For Raspberry Pi</t>
+  </si>
+  <si>
+    <t>CONHD-330060</t>
+  </si>
+  <si>
+    <t>CONPH-402749</t>
   </si>
 </sst>
 </file>
@@ -211,18 +232,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -505,348 +526,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6" style="5" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>99.99</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>7.1</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>14.4</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>16.989999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="5" t="s">
-        <v>29</v>
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2</v>
       </c>
       <c r="G8" s="6">
-        <f>SUM(G4:G7)</f>
-        <v>138.47999999999999</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="5" t="s">
-        <v>7</v>
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
       </c>
       <c r="G9" s="6">
-        <f>G8*0.13</f>
-        <v>18.002399999999998</v>
+        <v>6.89</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="5">
+        <f>SUM(G4:G9)</f>
+        <v>147.14999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="5">
+        <f>G10*0.13</f>
+        <v>19.129499999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="6">
-        <f>SUM(G8:G9)</f>
-        <v>156.48239999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9" t="s">
+      <c r="G12" s="5">
+        <f>SUM(G10:G11)</f>
+        <v>166.27949999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Necessary Stuff for Presentation
</commit_message>
<xml_diff>
--- a/2018_Documentation/Proposal, Budget, Project Schedule/Budget.xlsx
+++ b/2018_Documentation/Proposal, Budget, Project Schedule/Budget.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>No</t>
   </si>
@@ -130,14 +130,16 @@
   </si>
   <si>
     <t>CONPH-402749</t>
+  </si>
+  <si>
+    <t>Total shipping fee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+  <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -227,14 +229,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -526,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -538,32 +539,32 @@
     <col min="2" max="2" width="26.21875" style="4" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="17.109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
@@ -676,7 +677,7 @@
       <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>16.989999999999998</v>
       </c>
     </row>
@@ -699,7 +700,7 @@
       <c r="F8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>1.78</v>
       </c>
     </row>
@@ -722,7 +723,7 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>6.89</v>
       </c>
     </row>
@@ -730,14 +731,13 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="4"/>
       <c r="G10" s="5">
-        <f>SUM(G4:G9)</f>
-        <v>147.14999999999998</v>
+        <v>19.96</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -747,11 +747,11 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="G11" s="5">
-        <f>G10*0.13</f>
-        <v>19.129499999999997</v>
+        <f>SUM(G4:G10)</f>
+        <v>167.10999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -761,159 +761,173 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="5">
+        <f>G11*0.13</f>
+        <v>21.724299999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="5">
-        <f>SUM(G10:G11)</f>
-        <v>166.27949999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="G13" s="5">
+        <f>SUM(G11:G12)</f>
+        <v>188.83429999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>